<commit_message>
Will now consolidate bar onlys into bar when making comp summary
</commit_message>
<xml_diff>
--- a/scripts/Report_Templates/Summaries/CDP_Comp_Summary_Template.xlsx
+++ b/scripts/Report_Templates/Summaries/CDP_Comp_Summary_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zelda\Desktop\Work\ISIAL\SalesReportingAutomation\SalesReportAutomationProduct\scripts\Report_Templates\Summaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C18B65C-F0FE-4CC8-81CF-8E84E2D3C142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D2A107-EFA3-4FEB-BEFD-458E8E7B5F15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9495" yWindow="-21600" windowWidth="19410" windowHeight="20985" tabRatio="732" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="732" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Comp. Summary" sheetId="10" r:id="rId1"/>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>Total Covers</t>
   </si>
@@ -186,18 +186,9 @@
     <t>LUNCH &amp; DINNER SALES REPORT (Rolling N-Week)</t>
   </si>
   <si>
-    <t>Alcohol</t>
-  </si>
-  <si>
-    <t>Water</t>
-  </si>
-  <si>
     <t>Total Covers (Adj.)</t>
   </si>
   <si>
-    <t>Non-Alcohol</t>
-  </si>
-  <si>
     <t>Budget</t>
   </si>
   <si>
@@ -205,6 +196,9 @@
   </si>
   <si>
     <t>Total covers</t>
+  </si>
+  <si>
+    <t>Bar</t>
   </si>
 </sst>
 </file>
@@ -218,7 +212,7 @@
     <numFmt numFmtId="166" formatCode="0.0%"/>
     <numFmt numFmtId="167" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -514,15 +508,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
@@ -959,13 +953,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:S50"/>
+  <dimension ref="A1:S48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:A46"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="81" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" outlineLevelRow="1"/>
+  <sheetFormatPr defaultRowHeight="14" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.1796875" customWidth="1"/>
@@ -979,34 +973,34 @@
     <col min="13" max="19" width="13.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="36.5" customHeight="1"/>
-    <row r="2" spans="1:10" ht="18.5">
+    <row r="1" spans="1:10" ht="36.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2" s="10"/>
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-    </row>
-    <row r="3" spans="1:10" ht="19" thickBot="1">
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-    </row>
-    <row r="4" spans="1:10" ht="7.5" customHeight="1">
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+    </row>
+    <row r="3" spans="1:10" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+    </row>
+    <row r="4" spans="1:10" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="11"/>
     </row>
-    <row r="5" spans="1:10" ht="14.5">
+    <row r="5" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="13"/>
       <c r="C5" s="12"/>
@@ -1017,8 +1011,8 @@
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="14.5">
-      <c r="A6" s="47" t="s">
+    <row r="6" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="45" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="25"/>
@@ -1030,9 +1024,9 @@
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
     </row>
-    <row r="7" spans="1:10" ht="14.5">
-      <c r="A7" s="47" t="s">
-        <v>32</v>
+    <row r="7" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="45" t="s">
+        <v>30</v>
       </c>
       <c r="B7" s="27"/>
       <c r="C7" s="28"/>
@@ -1043,7 +1037,7 @@
       <c r="H7" s="28"/>
       <c r="I7" s="28"/>
     </row>
-    <row r="8" spans="1:10" ht="14.5">
+    <row r="8" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A8" s="37" t="s">
         <v>24</v>
       </c>
@@ -1056,7 +1050,7 @@
       <c r="H8" s="28"/>
       <c r="I8" s="28"/>
     </row>
-    <row r="9" spans="1:10" ht="14.5">
+    <row r="9" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A9" s="37" t="s">
         <v>25</v>
       </c>
@@ -1069,7 +1063,7 @@
       <c r="H9" s="28"/>
       <c r="I9" s="28"/>
     </row>
-    <row r="10" spans="1:10" ht="14.5">
+    <row r="10" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
         <v>28</v>
       </c>
@@ -1082,7 +1076,7 @@
       <c r="H10" s="28"/>
       <c r="I10" s="28"/>
     </row>
-    <row r="11" spans="1:10" ht="14.5">
+    <row r="11" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A11" s="37" t="s">
         <v>13</v>
       </c>
@@ -1095,7 +1089,7 @@
       <c r="H11" s="30"/>
       <c r="I11" s="30"/>
     </row>
-    <row r="12" spans="1:10" ht="14.5">
+    <row r="12" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A12" s="39" t="s">
         <v>1</v>
       </c>
@@ -1108,7 +1102,7 @@
       <c r="H12" s="30"/>
       <c r="I12" s="30"/>
     </row>
-    <row r="13" spans="1:10" ht="14.5">
+    <row r="13" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" s="42" t="s">
         <v>2</v>
       </c>
@@ -1121,7 +1115,7 @@
       <c r="H13" s="32"/>
       <c r="I13" s="32"/>
     </row>
-    <row r="14" spans="1:10" ht="14.5" outlineLevel="1">
+    <row r="14" spans="1:10" ht="14.5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="33"/>
       <c r="C14" s="34"/>
@@ -1132,7 +1126,7 @@
       <c r="H14" s="34"/>
       <c r="I14" s="34"/>
     </row>
-    <row r="15" spans="1:10" ht="14.5" outlineLevel="1">
+    <row r="15" spans="1:10" ht="14.5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A15" s="38" t="s">
         <v>26</v>
       </c>
@@ -1145,7 +1139,7 @@
       <c r="H15" s="34"/>
       <c r="I15" s="34"/>
     </row>
-    <row r="16" spans="1:10" ht="14.5">
+    <row r="16" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A16" s="38" t="s">
         <v>27</v>
       </c>
@@ -1158,7 +1152,7 @@
       <c r="H16" s="34"/>
       <c r="I16" s="34"/>
     </row>
-    <row r="17" spans="1:9" ht="14.5">
+    <row r="17" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A17" s="38" t="s">
         <v>14</v>
       </c>
@@ -1171,7 +1165,7 @@
       <c r="H17" s="34"/>
       <c r="I17" s="34"/>
     </row>
-    <row r="18" spans="1:9" ht="14.5">
+    <row r="18" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A18" s="40" t="s">
         <v>3</v>
       </c>
@@ -1184,7 +1178,7 @@
       <c r="H18" s="34"/>
       <c r="I18" s="34"/>
     </row>
-    <row r="19" spans="1:9" ht="14.5">
+    <row r="19" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A19" s="41" t="s">
         <v>4</v>
       </c>
@@ -1197,8 +1191,8 @@
       <c r="H19" s="35"/>
       <c r="I19" s="35"/>
     </row>
-    <row r="20" spans="1:9" ht="9.75" customHeight="1">
-      <c r="A20" s="47" t="s">
+    <row r="20" spans="1:9" ht="9.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="45" t="s">
         <v>5</v>
       </c>
       <c r="B20" s="15"/>
@@ -1210,7 +1204,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" ht="14.5">
+    <row r="21" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="16"/>
       <c r="C21" s="17"/>
@@ -1221,7 +1215,7 @@
       <c r="H21" s="17"/>
       <c r="I21" s="17"/>
     </row>
-    <row r="22" spans="1:9" ht="14.5">
+    <row r="22" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
@@ -1234,9 +1228,9 @@
       <c r="H22" s="17"/>
       <c r="I22" s="17"/>
     </row>
-    <row r="23" spans="1:9" ht="14.5">
+    <row r="23" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B23" s="16"/>
       <c r="C23" s="17"/>
@@ -1247,9 +1241,9 @@
       <c r="H23" s="17"/>
       <c r="I23" s="17"/>
     </row>
-    <row r="24" spans="1:9" ht="14.5">
+    <row r="24" spans="1:9" ht="14.5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="B24" s="16"/>
       <c r="C24" s="17"/>
@@ -1260,9 +1254,9 @@
       <c r="H24" s="17"/>
       <c r="I24" s="17"/>
     </row>
-    <row r="25" spans="1:9" ht="14.5">
+    <row r="25" spans="1:9" ht="14.5" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="B25" s="16"/>
       <c r="C25" s="17"/>
@@ -1273,9 +1267,9 @@
       <c r="H25" s="17"/>
       <c r="I25" s="17"/>
     </row>
-    <row r="26" spans="1:9" ht="14.5" outlineLevel="1">
+    <row r="26" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B26" s="16"/>
       <c r="C26" s="17"/>
@@ -1286,48 +1280,48 @@
       <c r="H26" s="17"/>
       <c r="I26" s="17"/>
     </row>
-    <row r="27" spans="1:9" ht="14.5" outlineLevel="1">
+    <row r="27" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B27" s="16"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="17"/>
-    </row>
-    <row r="28" spans="1:9" ht="14.5">
-      <c r="A28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B28" s="16"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="17"/>
-    </row>
-    <row r="29" spans="1:9" ht="14.5">
-      <c r="A29" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="15"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-    </row>
-    <row r="30" spans="1:9" ht="14.5">
-      <c r="A30" s="47" t="s">
+      <c r="B27" s="15"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="45" t="s">
         <v>5</v>
+      </c>
+      <c r="B28" s="20"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+    </row>
+    <row r="29" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="20"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+    </row>
+    <row r="30" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="43" t="s">
+        <v>32</v>
       </c>
       <c r="B30" s="20"/>
       <c r="C30" s="19"/>
@@ -1338,10 +1332,7 @@
       <c r="H30" s="19"/>
       <c r="I30" s="19"/>
     </row>
-    <row r="31" spans="1:9" ht="14.5">
-      <c r="A31" s="42" t="s">
-        <v>34</v>
-      </c>
+    <row r="31" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B31" s="20"/>
       <c r="C31" s="19"/>
       <c r="D31" s="19"/>
@@ -1351,45 +1342,48 @@
       <c r="H31" s="19"/>
       <c r="I31" s="19"/>
     </row>
-    <row r="32" spans="1:9" ht="14.5">
+    <row r="32" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A32" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="B32" s="20"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
-    </row>
-    <row r="33" spans="1:19" ht="14.5">
-      <c r="B33" s="20"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
-    </row>
-    <row r="34" spans="1:19" ht="14.5">
-      <c r="A34" s="47" t="s">
-        <v>36</v>
-      </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-    </row>
-    <row r="35" spans="1:19" ht="14.5">
-      <c r="A35" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="18"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+    </row>
+    <row r="33" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="B33" s="18"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+    </row>
+    <row r="34" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" s="21"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="22"/>
+    </row>
+    <row r="35" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="44" t="s">
+        <v>17</v>
       </c>
       <c r="B35" s="18"/>
       <c r="C35" s="2"/>
@@ -1400,12 +1394,12 @@
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
     </row>
-    <row r="36" spans="1:19" ht="14.5">
-      <c r="A36" s="46" t="s">
-        <v>16</v>
+    <row r="36" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A36" s="44" t="s">
+        <v>18</v>
       </c>
       <c r="B36" s="21"/>
-      <c r="C36" s="24"/>
+      <c r="C36" s="22"/>
       <c r="D36" s="22"/>
       <c r="E36" s="22"/>
       <c r="F36" s="22"/>
@@ -1413,9 +1407,9 @@
       <c r="H36" s="22"/>
       <c r="I36" s="22"/>
     </row>
-    <row r="37" spans="1:19" ht="14.5">
-      <c r="A37" s="46" t="s">
-        <v>17</v>
+    <row r="37" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="44" t="s">
+        <v>19</v>
       </c>
       <c r="B37" s="18"/>
       <c r="C37" s="2"/>
@@ -1426,9 +1420,9 @@
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
     </row>
-    <row r="38" spans="1:19" ht="14.5">
-      <c r="A38" s="46" t="s">
-        <v>18</v>
+    <row r="38" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="B38" s="21"/>
       <c r="C38" s="22"/>
@@ -1439,91 +1433,65 @@
       <c r="H38" s="22"/>
       <c r="I38" s="22"/>
     </row>
-    <row r="39" spans="1:19" ht="14.5">
-      <c r="A39" s="46" t="s">
-        <v>19</v>
-      </c>
-      <c r="B39" s="18"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-    </row>
-    <row r="40" spans="1:19" ht="14.5">
-      <c r="A40" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B40" s="21"/>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
-      <c r="H40" s="22"/>
-      <c r="I40" s="22"/>
-    </row>
-    <row r="41" spans="1:19" ht="15" thickBot="1">
+    <row r="39" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" s="23"/>
+    </row>
+    <row r="40" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="J40" s="1"/>
+    </row>
+    <row r="41" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B41" s="23"/>
-    </row>
-    <row r="42" spans="1:19" ht="14.5">
-      <c r="A42" s="46" t="s">
-        <v>10</v>
-      </c>
-      <c r="J42" s="1"/>
-    </row>
-    <row r="43" spans="1:19" ht="14.5">
+        <v>20</v>
+      </c>
+      <c r="B41" s="5"/>
+      <c r="K41" s="4"/>
+    </row>
+    <row r="42" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A42" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" s="6"/>
+      <c r="K42" s="1"/>
+      <c r="M42" s="9"/>
+      <c r="N42" s="9"/>
+      <c r="O42" s="9"/>
+      <c r="P42" s="9"/>
+      <c r="Q42" s="9"/>
+      <c r="R42" s="9"/>
+      <c r="S42" s="9"/>
+    </row>
+    <row r="43" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B43" s="5"/>
-      <c r="K43" s="4"/>
-    </row>
-    <row r="44" spans="1:19" ht="14.5">
-      <c r="A44" s="46" t="s">
-        <v>22</v>
-      </c>
-      <c r="B44" s="6"/>
-      <c r="K44" s="1"/>
-      <c r="M44" s="9"/>
-      <c r="N44" s="9"/>
-      <c r="O44" s="9"/>
-      <c r="P44" s="9"/>
-      <c r="Q44" s="9"/>
-      <c r="R44" s="9"/>
-      <c r="S44" s="9"/>
-    </row>
-    <row r="45" spans="1:19" ht="14.5">
-      <c r="A45" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="14.5">
-      <c r="A46" s="46" t="s">
+    <row r="44" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A44" s="44" t="s">
         <v>23</v>
       </c>
+      <c r="C44" s="3"/>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B45" s="7"/>
+      <c r="C45" s="3"/>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B46" s="7"/>
       <c r="C46" s="3"/>
     </row>
-    <row r="47" spans="1:19">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B47" s="7"/>
       <c r="C47" s="3"/>
     </row>
-    <row r="48" spans="1:19">
-      <c r="B48" s="7"/>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B48" s="8"/>
       <c r="C48" s="3"/>
-    </row>
-    <row r="49" spans="2:3">
-      <c r="B49" s="7"/>
-      <c r="C49" s="3"/>
-    </row>
-    <row r="50" spans="2:3">
-      <c r="B50" s="8"/>
-      <c r="C50" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>